<commit_message>
some excel import fixes
</commit_message>
<xml_diff>
--- a/src/assets/parcelTemplate.xlsx
+++ b/src/assets/parcelTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\home\Desktop\New folder (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\home\IdeaProjects\Delivery\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>მიმღები</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>კარტოშკა</t>
+  </si>
+  <si>
+    <t>123456789</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,8 +478,8 @@
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
-        <v>11001028583</v>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>11</v>

</xml_diff>